<commit_message>
Agregado el documento para impresión de la entrega 1. Correciones menores.
</commit_message>
<xml_diff>
--- a/SAP - TECNOLOGIA/Iteración I/01 - Análisis de Requerimientos/02 - Requerimientos/Requerimientos No Funcionales 1.1.xlsx
+++ b/SAP - TECNOLOGIA/Iteración I/01 - Análisis de Requerimientos/02 - Requerimientos/Requerimientos No Funcionales 1.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\SAP-TFI 2015\sap-tfi-documentation\SAP - TECNOLOGIA\Inicio del Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\SAP-TFI 2015\sap-tfi-documentation\SAP - TECNOLOGIA\Iteración I\01 - Análisis de Requerimientos\02 - Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -162,7 +162,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -170,14 +170,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -491,7 +508,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,50 +519,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>